<commit_message>
Solved world age issue
Created a single file that includes all the others. Turned the other includes into comments. This prevents an error with different world ages. Also changed it in the README
</commit_message>
<xml_diff>
--- a/planning/start_up.xlsx
+++ b/planning/start_up.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d09dd78596f01afe/Bureaublad/IbM-2.4.3/IbM-2.4.3/planning/Excels/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsbie\Documents\Universiteit\Master\Jaar 2\MEP\Code\IbM-Fermentation\IbM-Fermentation\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAA9B15-575C-4149-BBBA-251812EBF2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A036797D-EE45-49D3-9F81-A7F690DE219E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="0" windowWidth="17250" windowHeight="8865" tabRatio="808" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10950" yWindow="-15705" windowWidth="17220" windowHeight="8850" tabRatio="808" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="279">
   <si>
     <t>AOB/AOA</t>
   </si>
@@ -1339,18 +1339,12 @@
     <t>Average expected radius of all granules</t>
   </si>
   <si>
-    <t>density granule</t>
-  </si>
-  <si>
     <t>g/L</t>
   </si>
   <si>
     <t>How dense are the granules</t>
   </si>
   <si>
-    <t>density reactor</t>
-  </si>
-  <si>
     <t>How much biomass (at most) is in the reactor</t>
   </si>
   <si>
@@ -1409,6 +1403,15 @@
   </si>
   <si>
     <t>Add columns with per bacterial species the Ks values [M] per substrate. Make sure that the compound and bacterium names match the rest of the Excel file</t>
+  </si>
+  <si>
+    <t>Currently this is a copy of granule_template, but with reduced simulation time</t>
+  </si>
+  <si>
+    <t>Density granule</t>
+  </si>
+  <si>
+    <t>Density reactor</t>
   </si>
 </sst>
 </file>
@@ -4285,7 +4288,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B1" s="121">
         <f>Influent!B1/2</f>
@@ -4303,7 +4306,7 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B2" s="121">
         <f>Influent!B2/2</f>
@@ -4461,7 +4464,7 @@
     </row>
     <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B2" s="151" t="s">
         <v>85</v>
@@ -4490,7 +4493,7 @@
     </row>
     <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B3" s="151" t="s">
         <v>85</v>
@@ -4751,7 +4754,7 @@
     </row>
     <row r="13" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="76" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B13" s="103">
         <f>IF(COUNT(B2,C2)=2, EXP(($C$10+B2-C2)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
@@ -4776,7 +4779,7 @@
     </row>
     <row r="14" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B14" s="103">
         <f>IF(COUNT(B3,C3)=2, EXP(($C$10+B3-C3)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
@@ -4992,7 +4995,7 @@
     </row>
     <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B24" s="152" t="s">
         <v>86</v>
@@ -5015,7 +5018,7 @@
     </row>
     <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="77" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B25" s="152" t="s">
         <v>86</v>
@@ -5269,10 +5272,10 @@
     <row r="1" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="64"/>
       <c r="B1" s="136" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C1" s="136" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D1" s="136" t="s">
         <v>17</v>
@@ -5281,12 +5284,12 @@
         <v>76</v>
       </c>
       <c r="F1" s="275" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B2" s="100">
         <v>1.0000000000000001E-5</v>
@@ -5304,7 +5307,7 @@
     </row>
     <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B3" s="100">
         <v>0</v>
@@ -5322,7 +5325,7 @@
     </row>
     <row r="4" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B4" s="100">
         <v>0</v>
@@ -5376,21 +5379,21 @@
     <row r="1" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="64"/>
       <c r="B1" s="136" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C1" s="136" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D1" s="136" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="275" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B2" s="100">
         <v>0</v>
@@ -5405,7 +5408,7 @@
     </row>
     <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B3" s="100">
         <v>0</v>
@@ -5420,7 +5423,7 @@
     </row>
     <row r="4" spans="1:5" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B4" s="100">
         <v>0</v>
@@ -5478,18 +5481,18 @@
         <v>226</v>
       </c>
       <c r="F1" s="270" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B2" s="100">
         <v>0.01</v>
       </c>
       <c r="C2" s="137" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D2" s="138">
         <f>0.25/24</f>
@@ -5503,13 +5506,13 @@
     </row>
     <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B3" s="100">
         <v>0.01</v>
       </c>
       <c r="C3" s="137" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D3" s="138">
         <f>0.25/24</f>
@@ -5523,7 +5526,7 @@
     </row>
     <row r="4" spans="1:6" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B4" s="100">
         <v>0.01</v>
@@ -5574,17 +5577,17 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="69"/>
       <c r="B1" s="276" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C1" s="277"/>
       <c r="D1" s="278"/>
       <c r="E1" s="276" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F1" s="277"/>
       <c r="G1" s="278"/>
       <c r="H1" s="277" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I1" s="277"/>
       <c r="J1" s="278"/>
@@ -5621,7 +5624,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="76" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B3" s="164">
         <v>-1</v>
@@ -5653,7 +5656,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B4" s="166">
         <v>0</v>
@@ -8462,7 +8465,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8588,6 +8591,9 @@
       <c r="C11" s="173"/>
     </row>
     <row r="12" spans="1:3" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>276</v>
+      </c>
       <c r="C12" s="173"/>
     </row>
     <row r="13" spans="1:3" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -8612,8 +8618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8756,7 +8762,7 @@
         <v>121</v>
       </c>
       <c r="B9" s="102">
-        <v>3600</v>
+        <v>10</v>
       </c>
       <c r="C9" s="91" t="s">
         <v>93</v>
@@ -8904,7 +8910,7 @@
         <v>90</v>
       </c>
       <c r="D18" s="107" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E18" s="264"/>
     </row>
@@ -9022,10 +9028,10 @@
         <v>0.2</v>
       </c>
       <c r="C26" s="90" t="s">
+        <v>263</v>
+      </c>
+      <c r="D26" s="112" t="s">
         <v>265</v>
-      </c>
-      <c r="D26" s="112" t="s">
-        <v>267</v>
       </c>
       <c r="E26" s="264"/>
     </row>
@@ -9037,10 +9043,10 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="C27" s="90" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D27" s="112" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E27" s="264"/>
     </row>
@@ -9084,8 +9090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9148,7 +9154,7 @@
         <v>161</v>
       </c>
       <c r="B4" s="106" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C4" s="119" t="s">
         <v>90</v>
@@ -9252,31 +9258,31 @@
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="77" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="B11" s="225">
         <v>100</v>
       </c>
       <c r="C11" s="90" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" s="226" t="s">
         <v>255</v>
-      </c>
-      <c r="D11" s="226" t="s">
-        <v>256</v>
       </c>
       <c r="E11" s="69"/>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="89" t="s">
-        <v>257</v>
+        <v>278</v>
       </c>
       <c r="B12" s="227">
         <v>3</v>
       </c>
       <c r="C12" s="92" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D12" s="228" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E12" s="69"/>
     </row>
@@ -9417,7 +9423,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B1" s="116">
         <f>1*10^(-9)*3600</f>
@@ -9435,7 +9441,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="77" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B2" s="116">
         <f>1*10^(-9)*3600</f>
@@ -9662,7 +9668,7 @@
         <v>90</v>
       </c>
       <c r="D6" s="232" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -9697,7 +9703,7 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="174" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B9" s="122">
         <v>12</v>
@@ -9706,12 +9712,12 @@
         <v>90</v>
       </c>
       <c r="D9" s="233" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="234" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B10" s="186">
         <v>12</v>
@@ -9720,7 +9726,7 @@
         <v>90</v>
       </c>
       <c r="D10" s="235" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -9770,7 +9776,7 @@
         <v>187</v>
       </c>
       <c r="B14" s="128" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C14" s="129" t="s">
         <v>90</v>
@@ -9864,8 +9870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9966,10 +9972,10 @@
         <v>0.05</v>
       </c>
       <c r="C7" s="90" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D7" s="231" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -10087,7 +10093,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B1" s="121">
         <f>2*Parameters!B3</f>
@@ -10110,7 +10116,7 @@
     </row>
     <row r="2" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B2" s="121">
         <f>2*Parameters!B3</f>

</xml_diff>